<commit_message>
changed the mark points
</commit_message>
<xml_diff>
--- a/FOV_of_Interest.xlsx
+++ b/FOV_of_Interest.xlsx
@@ -281,10 +281,10 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
@@ -377,10 +377,10 @@
         <v>16</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -400,10 +400,10 @@
         <v>20</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N5" s="3" t="s">
         <v>12</v>
@@ -429,10 +429,10 @@
         <v>35</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N6" s="0" t="s">
         <v>16</v>
@@ -461,10 +461,10 @@
         <v>15</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="N7" s="3" t="s">
         <v>20</v>
@@ -493,10 +493,10 @@
         <v>59</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -516,10 +516,10 @@
         <v>97</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -539,10 +539,10 @@
         <v>11</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -562,10 +562,10 @@
         <v>11</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -585,10 +585,10 @@
         <v>12</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>